<commit_message>
update price in fuel consumtion
</commit_message>
<xml_diff>
--- a/public/assets/import/Format Import Fuel Consumtion.xlsx
+++ b/public/assets/import/Format Import Fuel Consumtion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADI\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADI\Herd\real_management_asset\public\assets\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0E988A-0548-4261-920F-D176B0E67542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59B63A4-C272-4C53-BFD9-D066E1062F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA1D98C6-E154-4961-BE6A-65DFD75615DE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>asset_id</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>liter</t>
-  </si>
-  <si>
-    <t>price</t>
   </si>
   <si>
     <t>category</t>
@@ -573,28 +570,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7D2908-82AD-4939-883C-E3BFE070B16E}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" style="2" customWidth="1"/>
-    <col min="2" max="9" width="21.7109375" style="2"/>
-    <col min="10" max="16384" width="21.7109375" style="1"/>
+    <col min="2" max="8" width="21.7109375" style="2"/>
+    <col min="9" max="16384" width="21.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -611,326 +608,290 @@
       <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45644</v>
+      </c>
+      <c r="E2" s="2">
+        <v>100</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H2" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3">
-        <v>45644</v>
-      </c>
-      <c r="E2" s="2">
-        <v>100</v>
-      </c>
-      <c r="F2" s="2">
-        <v>12000</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45644</v>
+      </c>
+      <c r="E3" s="2">
+        <v>100</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I2" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="G3" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H3" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3">
-        <v>45644</v>
-      </c>
-      <c r="E3" s="2">
-        <v>100</v>
-      </c>
-      <c r="F3" s="2">
-        <v>12000</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="D4" s="3">
+        <v>45644</v>
+      </c>
+      <c r="E4" s="2">
+        <v>100</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I3" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="G4" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H4" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3">
-        <v>45644</v>
-      </c>
-      <c r="E4" s="2">
-        <v>100</v>
-      </c>
-      <c r="F4" s="2">
-        <v>12000</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="D5" s="3">
+        <v>45644</v>
+      </c>
+      <c r="E5" s="2">
+        <v>100</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I4" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="G5" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3">
-        <v>45644</v>
-      </c>
-      <c r="E5" s="2">
-        <v>100</v>
-      </c>
-      <c r="F5" s="2">
-        <v>12000</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="D6" s="3">
+        <v>45644</v>
+      </c>
+      <c r="E6" s="2">
+        <v>100</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I5" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="G6" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H6" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3">
-        <v>45644</v>
-      </c>
-      <c r="E6" s="2">
-        <v>100</v>
-      </c>
-      <c r="F6" s="2">
-        <v>12000</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="D7" s="3">
+        <v>45644</v>
+      </c>
+      <c r="E7" s="2">
+        <v>100</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I6" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="G7" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3">
-        <v>45644</v>
-      </c>
-      <c r="E7" s="2">
-        <v>100</v>
-      </c>
-      <c r="F7" s="2">
-        <v>12000</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="D8" s="3">
+        <v>45644</v>
+      </c>
+      <c r="E8" s="2">
+        <v>100</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I7" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="G8" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H8" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="3">
-        <v>45644</v>
-      </c>
-      <c r="E8" s="2">
-        <v>100</v>
-      </c>
-      <c r="F8" s="2">
-        <v>12000</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="D9" s="3">
+        <v>45644</v>
+      </c>
+      <c r="E9" s="2">
+        <v>100</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I8" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="G9" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H9" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3">
-        <v>45644</v>
-      </c>
-      <c r="E9" s="2">
-        <v>100</v>
-      </c>
-      <c r="F9" s="2">
-        <v>12000</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="D10" s="3">
+        <v>45644</v>
+      </c>
+      <c r="E10" s="2">
+        <v>100</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I9" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="G10" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H10" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="3">
-        <v>45644</v>
-      </c>
-      <c r="E10" s="2">
-        <v>100</v>
-      </c>
-      <c r="F10" s="2">
-        <v>12000</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="D11" s="3">
+        <v>45644</v>
+      </c>
+      <c r="E11" s="2">
+        <v>100</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I10" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="G11" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="3">
-        <v>45644</v>
-      </c>
-      <c r="E11" s="2">
-        <v>100</v>
-      </c>
-      <c r="F11" s="2">
-        <v>12000</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="D12" s="3">
+        <v>45644</v>
+      </c>
+      <c r="E12" s="2">
+        <v>100</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I11" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="3">
-        <v>45644</v>
-      </c>
-      <c r="E12" s="2">
-        <v>100</v>
-      </c>
-      <c r="F12" s="2">
-        <v>12000</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>42</v>
+      <c r="G12" s="2">
+        <v>100000</v>
       </c>
       <c r="H12" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I12" s="2">
         <v>10</v>
       </c>
     </row>

</xml_diff>